<commit_message>
fix: fixed formatting when scrapping floating point numbers
</commit_message>
<xml_diff>
--- a/contratos/contratos-1-2009.xlsx
+++ b/contratos/contratos-1-2009.xlsx
@@ -571,7 +571,7 @@
     <t>IGLESIAS JOSE FABIAN</t>
   </si>
   <si>
-    <t>PITTER ROLANDO L.J, CERGNEUX MARIO M. Y CERGNEUX DANIEL F.  S.H.</t>
+    <t>PITTER ROLANDO LJ. CERGNEUX MARIO M Y CERGNEUX DANIEL F  SH</t>
   </si>
   <si>
     <t>SYLVESTRE CARLOS OMAR</t>
@@ -589,16 +589,16 @@
     <t>CIVITAS S.A.</t>
   </si>
   <si>
-    <t>FERNANDEZ MARIO H, GALLICET OSCAR M</t>
-  </si>
-  <si>
-    <t>IZAGUIRRE CARLOS MARIA, MOREND MARIA ELENA Y MOREND MARIA TERESA</t>
+    <t>FERNANDEZ MARIO H. GALLICET OSCAR M</t>
+  </si>
+  <si>
+    <t>IZAGUIRRE CARLOS MARIA. MOREND MARIA ELENA Y MOREND MARIA TERESA</t>
   </si>
   <si>
     <t>LEIVA GISELA NOEMI</t>
   </si>
   <si>
-    <t>MARSICO GUILLERMO MIGUEL, MARSICO JUAN EDUARDO</t>
+    <t>MARSICO GUILLERMO MIGUEL. MARSICO JUAN EDUARDO</t>
   </si>
   <si>
     <t>OLIVERA JOSE PEDRO</t>
@@ -622,7 +622,7 @@
     <t>JUSID NICOLAS</t>
   </si>
   <si>
-    <t>RICCOTTI, MARIANA EDITH</t>
+    <t>RICCOTTI. MARIANA EDITH</t>
   </si>
   <si>
     <t>STEVEN MIGUEL ANGEL</t>
@@ -994,373 +994,373 @@
     <t>214</t>
   </si>
   <si>
-    <t>770,00</t>
-  </si>
-  <si>
-    <t>2.471,15</t>
-  </si>
-  <si>
-    <t>22.423,54</t>
-  </si>
-  <si>
-    <t>3.223,14</t>
-  </si>
-  <si>
-    <t>410,00</t>
-  </si>
-  <si>
-    <t>25.560,00</t>
-  </si>
-  <si>
-    <t>88.796,58</t>
-  </si>
-  <si>
-    <t>12.857,11</t>
-  </si>
-  <si>
-    <t>349,04</t>
-  </si>
-  <si>
-    <t>1.796,10</t>
-  </si>
-  <si>
-    <t>2.377,54</t>
-  </si>
-  <si>
-    <t>1.111,00</t>
-  </si>
-  <si>
-    <t>5.347,83</t>
-  </si>
-  <si>
-    <t>80,00</t>
-  </si>
-  <si>
-    <t>667,00</t>
-  </si>
-  <si>
-    <t>10.636,49</t>
-  </si>
-  <si>
-    <t>1.650,00</t>
-  </si>
-  <si>
-    <t>3.040,00</t>
-  </si>
-  <si>
-    <t>143,00</t>
-  </si>
-  <si>
-    <t>332,50</t>
-  </si>
-  <si>
-    <t>483,65</t>
-  </si>
-  <si>
-    <t>482,13</t>
-  </si>
-  <si>
-    <t>18.303,22</t>
-  </si>
-  <si>
-    <t>5.970,99</t>
-  </si>
-  <si>
-    <t>1.413,90</t>
-  </si>
-  <si>
-    <t>74,40</t>
-  </si>
-  <si>
-    <t>7.553,00</t>
-  </si>
-  <si>
-    <t>14,08</t>
-  </si>
-  <si>
-    <t>799,50</t>
-  </si>
-  <si>
-    <t>71,10</t>
-  </si>
-  <si>
-    <t>135,00</t>
-  </si>
-  <si>
-    <t>800,50</t>
-  </si>
-  <si>
-    <t>99,00</t>
-  </si>
-  <si>
-    <t>2.139,00</t>
-  </si>
-  <si>
-    <t>966,00</t>
-  </si>
-  <si>
-    <t>986,50</t>
-  </si>
-  <si>
-    <t>825,00</t>
-  </si>
-  <si>
-    <t>374,00</t>
-  </si>
-  <si>
-    <t>126,54</t>
-  </si>
-  <si>
-    <t>83,60</t>
-  </si>
-  <si>
-    <t>1.600,00</t>
-  </si>
-  <si>
-    <t>1.592,00</t>
-  </si>
-  <si>
-    <t>1.495,00</t>
-  </si>
-  <si>
-    <t>459,80</t>
-  </si>
-  <si>
-    <t>509,00</t>
-  </si>
-  <si>
-    <t>1.700,00</t>
-  </si>
-  <si>
-    <t>54,00</t>
-  </si>
-  <si>
-    <t>17.182,80</t>
-  </si>
-  <si>
-    <t>5.540,00</t>
-  </si>
-  <si>
-    <t>2.394,00</t>
-  </si>
-  <si>
-    <t>329.410,00</t>
-  </si>
-  <si>
-    <t>302,00</t>
-  </si>
-  <si>
-    <t>29,25</t>
-  </si>
-  <si>
-    <t>2.300,08</t>
-  </si>
-  <si>
-    <t>280,00</t>
-  </si>
-  <si>
-    <t>1.318,00</t>
-  </si>
-  <si>
-    <t>45,00</t>
-  </si>
-  <si>
-    <t>560,00</t>
-  </si>
-  <si>
-    <t>680,00</t>
-  </si>
-  <si>
-    <t>190,00</t>
-  </si>
-  <si>
-    <t>213.732,00</t>
-  </si>
-  <si>
-    <t>4.564,46</t>
-  </si>
-  <si>
-    <t>1.544,63</t>
-  </si>
-  <si>
-    <t>455,73</t>
-  </si>
-  <si>
-    <t>1.009,92</t>
-  </si>
-  <si>
-    <t>19.919,18</t>
-  </si>
-  <si>
-    <t>12.119,38</t>
-  </si>
-  <si>
-    <t>510,20</t>
-  </si>
-  <si>
-    <t>27,00</t>
-  </si>
-  <si>
-    <t>3.601,50</t>
-  </si>
-  <si>
-    <t>4.481,43</t>
-  </si>
-  <si>
-    <t>182,65</t>
-  </si>
-  <si>
-    <t>99,64</t>
-  </si>
-  <si>
-    <t>10.000,00</t>
-  </si>
-  <si>
-    <t>520,00</t>
-  </si>
-  <si>
-    <t>1.238,00</t>
-  </si>
-  <si>
-    <t>1.200,00</t>
-  </si>
-  <si>
-    <t>4.132,23</t>
-  </si>
-  <si>
-    <t>6.000,00</t>
-  </si>
-  <si>
-    <t>230,00</t>
-  </si>
-  <si>
-    <t>400,00</t>
-  </si>
-  <si>
-    <t>124.988,05</t>
-  </si>
-  <si>
-    <t>4.125,00</t>
-  </si>
-  <si>
-    <t>1.400,00</t>
-  </si>
-  <si>
-    <t>16,00</t>
-  </si>
-  <si>
-    <t>504,50</t>
-  </si>
-  <si>
-    <t>1.367,45</t>
-  </si>
-  <si>
-    <t>236.726,79</t>
-  </si>
-  <si>
-    <t>10.500,00</t>
-  </si>
-  <si>
-    <t>220,00</t>
-  </si>
-  <si>
-    <t>1.675,00</t>
-  </si>
-  <si>
-    <t>650,00</t>
-  </si>
-  <si>
-    <t>5.745,24</t>
-  </si>
-  <si>
-    <t>200,00</t>
-  </si>
-  <si>
-    <t>250,00</t>
-  </si>
-  <si>
-    <t>2.500,00</t>
-  </si>
-  <si>
-    <t>25.000,00</t>
-  </si>
-  <si>
-    <t>120,00</t>
-  </si>
-  <si>
-    <t>7.969,35</t>
-  </si>
-  <si>
-    <t>85,00</t>
-  </si>
-  <si>
-    <t>50,00</t>
-  </si>
-  <si>
-    <t>20,00</t>
-  </si>
-  <si>
-    <t>95,00</t>
-  </si>
-  <si>
-    <t>125,00</t>
-  </si>
-  <si>
-    <t>1.065,00</t>
-  </si>
-  <si>
-    <t>987,36</t>
-  </si>
-  <si>
-    <t>3.798,62</t>
-  </si>
-  <si>
-    <t>425,00</t>
-  </si>
-  <si>
-    <t>215,10</t>
-  </si>
-  <si>
-    <t>736,00</t>
-  </si>
-  <si>
-    <t>75,00</t>
-  </si>
-  <si>
-    <t>10.002,20</t>
-  </si>
-  <si>
-    <t>952,38</t>
-  </si>
-  <si>
-    <t>19.282,12</t>
-  </si>
-  <si>
-    <t>2.360,00</t>
-  </si>
-  <si>
-    <t>477,75</t>
-  </si>
-  <si>
-    <t>2.913,00</t>
-  </si>
-  <si>
-    <t>8.625,00</t>
-  </si>
-  <si>
-    <t>729,25</t>
-  </si>
-  <si>
-    <t>2.124,20</t>
-  </si>
-  <si>
-    <t>3.890,00</t>
-  </si>
-  <si>
-    <t>530,00</t>
-  </si>
-  <si>
-    <t>450,00</t>
+    <t>770.00</t>
+  </si>
+  <si>
+    <t>2471.15</t>
+  </si>
+  <si>
+    <t>22423.54</t>
+  </si>
+  <si>
+    <t>3223.14</t>
+  </si>
+  <si>
+    <t>410.00</t>
+  </si>
+  <si>
+    <t>25560.00</t>
+  </si>
+  <si>
+    <t>88796.58</t>
+  </si>
+  <si>
+    <t>12857.11</t>
+  </si>
+  <si>
+    <t>349.04</t>
+  </si>
+  <si>
+    <t>1796.10</t>
+  </si>
+  <si>
+    <t>2377.54</t>
+  </si>
+  <si>
+    <t>1111.00</t>
+  </si>
+  <si>
+    <t>5347.83</t>
+  </si>
+  <si>
+    <t>80.00</t>
+  </si>
+  <si>
+    <t>667.00</t>
+  </si>
+  <si>
+    <t>10636.49</t>
+  </si>
+  <si>
+    <t>1650.00</t>
+  </si>
+  <si>
+    <t>3040.00</t>
+  </si>
+  <si>
+    <t>143.00</t>
+  </si>
+  <si>
+    <t>332.50</t>
+  </si>
+  <si>
+    <t>483.65</t>
+  </si>
+  <si>
+    <t>482.13</t>
+  </si>
+  <si>
+    <t>18303.22</t>
+  </si>
+  <si>
+    <t>5970.99</t>
+  </si>
+  <si>
+    <t>1413.90</t>
+  </si>
+  <si>
+    <t>74.40</t>
+  </si>
+  <si>
+    <t>7553.00</t>
+  </si>
+  <si>
+    <t>14.08</t>
+  </si>
+  <si>
+    <t>799.50</t>
+  </si>
+  <si>
+    <t>71.10</t>
+  </si>
+  <si>
+    <t>135.00</t>
+  </si>
+  <si>
+    <t>800.50</t>
+  </si>
+  <si>
+    <t>99.00</t>
+  </si>
+  <si>
+    <t>2139.00</t>
+  </si>
+  <si>
+    <t>966.00</t>
+  </si>
+  <si>
+    <t>986.50</t>
+  </si>
+  <si>
+    <t>825.00</t>
+  </si>
+  <si>
+    <t>374.00</t>
+  </si>
+  <si>
+    <t>126.54</t>
+  </si>
+  <si>
+    <t>83.60</t>
+  </si>
+  <si>
+    <t>1600.00</t>
+  </si>
+  <si>
+    <t>1592.00</t>
+  </si>
+  <si>
+    <t>1495.00</t>
+  </si>
+  <si>
+    <t>459.80</t>
+  </si>
+  <si>
+    <t>509.00</t>
+  </si>
+  <si>
+    <t>1700.00</t>
+  </si>
+  <si>
+    <t>54.00</t>
+  </si>
+  <si>
+    <t>17182.80</t>
+  </si>
+  <si>
+    <t>5540.00</t>
+  </si>
+  <si>
+    <t>2394.00</t>
+  </si>
+  <si>
+    <t>329410.00</t>
+  </si>
+  <si>
+    <t>302.00</t>
+  </si>
+  <si>
+    <t>29.25</t>
+  </si>
+  <si>
+    <t>2300.08</t>
+  </si>
+  <si>
+    <t>280.00</t>
+  </si>
+  <si>
+    <t>1318.00</t>
+  </si>
+  <si>
+    <t>45.00</t>
+  </si>
+  <si>
+    <t>560.00</t>
+  </si>
+  <si>
+    <t>680.00</t>
+  </si>
+  <si>
+    <t>190.00</t>
+  </si>
+  <si>
+    <t>213732.00</t>
+  </si>
+  <si>
+    <t>4564.46</t>
+  </si>
+  <si>
+    <t>1544.63</t>
+  </si>
+  <si>
+    <t>455.73</t>
+  </si>
+  <si>
+    <t>1009.92</t>
+  </si>
+  <si>
+    <t>19919.18</t>
+  </si>
+  <si>
+    <t>12119.38</t>
+  </si>
+  <si>
+    <t>510.20</t>
+  </si>
+  <si>
+    <t>27.00</t>
+  </si>
+  <si>
+    <t>3601.50</t>
+  </si>
+  <si>
+    <t>4481.43</t>
+  </si>
+  <si>
+    <t>182.65</t>
+  </si>
+  <si>
+    <t>99.64</t>
+  </si>
+  <si>
+    <t>10000.00</t>
+  </si>
+  <si>
+    <t>520.00</t>
+  </si>
+  <si>
+    <t>1238.00</t>
+  </si>
+  <si>
+    <t>1200.00</t>
+  </si>
+  <si>
+    <t>4132.23</t>
+  </si>
+  <si>
+    <t>6000.00</t>
+  </si>
+  <si>
+    <t>230.00</t>
+  </si>
+  <si>
+    <t>400.00</t>
+  </si>
+  <si>
+    <t>124988.05</t>
+  </si>
+  <si>
+    <t>4125.00</t>
+  </si>
+  <si>
+    <t>1400.00</t>
+  </si>
+  <si>
+    <t>16.00</t>
+  </si>
+  <si>
+    <t>504.50</t>
+  </si>
+  <si>
+    <t>1367.45</t>
+  </si>
+  <si>
+    <t>236726.79</t>
+  </si>
+  <si>
+    <t>10500.00</t>
+  </si>
+  <si>
+    <t>220.00</t>
+  </si>
+  <si>
+    <t>1675.00</t>
+  </si>
+  <si>
+    <t>650.00</t>
+  </si>
+  <si>
+    <t>5745.24</t>
+  </si>
+  <si>
+    <t>200.00</t>
+  </si>
+  <si>
+    <t>250.00</t>
+  </si>
+  <si>
+    <t>2500.00</t>
+  </si>
+  <si>
+    <t>25000.00</t>
+  </si>
+  <si>
+    <t>120.00</t>
+  </si>
+  <si>
+    <t>7969.35</t>
+  </si>
+  <si>
+    <t>85.00</t>
+  </si>
+  <si>
+    <t>50.00</t>
+  </si>
+  <si>
+    <t>20.00</t>
+  </si>
+  <si>
+    <t>95.00</t>
+  </si>
+  <si>
+    <t>125.00</t>
+  </si>
+  <si>
+    <t>1065.00</t>
+  </si>
+  <si>
+    <t>987.36</t>
+  </si>
+  <si>
+    <t>3798.62</t>
+  </si>
+  <si>
+    <t>425.00</t>
+  </si>
+  <si>
+    <t>215.10</t>
+  </si>
+  <si>
+    <t>736.00</t>
+  </si>
+  <si>
+    <t>75.00</t>
+  </si>
+  <si>
+    <t>10002.20</t>
+  </si>
+  <si>
+    <t>952.38</t>
+  </si>
+  <si>
+    <t>19282.12</t>
+  </si>
+  <si>
+    <t>2360.00</t>
+  </si>
+  <si>
+    <t>477.75</t>
+  </si>
+  <si>
+    <t>2913.00</t>
+  </si>
+  <si>
+    <t>8625.00</t>
+  </si>
+  <si>
+    <t>729.25</t>
+  </si>
+  <si>
+    <t>2124.20</t>
+  </si>
+  <si>
+    <t>3890.00</t>
+  </si>
+  <si>
+    <t>530.00</t>
+  </si>
+  <si>
+    <t>450.00</t>
   </si>
 </sst>
 </file>

</xml_diff>